<commit_message>
update analysis MPAs argument
</commit_message>
<xml_diff>
--- a/data/indicator_binning.xlsx
+++ b/data/indicator_binning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HarbinJ\Documents\GitHub\MarConsNetAnalysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96589E00-EAD3-42E3-A0AC-9A70A46A1422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86463E0-5FAC-451F-B179-4DB4BBA1998D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="178">
   <si>
     <t>indicators</t>
   </si>
@@ -965,7 +965,7 @@
     <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A68" sqref="A68"/>
-      <selection pane="topRight" activeCell="E114" sqref="E114"/>
+      <selection pane="topRight" activeCell="E90" sqref="E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2766,7 +2766,9 @@
       <c r="C90" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="D90" s="6"/>
+      <c r="D90" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="E90">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
update plots for indicators
</commit_message>
<xml_diff>
--- a/data/indicator_binning.xlsx
+++ b/data/indicator_binning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HarbinJ\Documents\GitHub\MarConsNetAnalysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0305980F-1504-40BA-BCA9-2BBA2AD7EBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5CD74A-0A43-496E-9B71-311829AD2600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="185">
   <si>
     <t>indicators</t>
   </si>
@@ -373,9 +373,6 @@
     <t>Distribution and abundance of seabird species within the MPA</t>
   </si>
   <si>
-    <t>Fish Condition</t>
-  </si>
-  <si>
     <t>Groundfish /commercial landings</t>
   </si>
   <si>
@@ -541,25 +538,46 @@
     <t>sea surface height</t>
   </si>
   <si>
-    <t>plot_azmp_physical(mpa=MPAs,parameter="nitrate", type="surface")</t>
-  </si>
-  <si>
-    <t>plot_azmp_physical(mpa=MPAs,parameter="salinity", type="surface", dataframe=TRUE)</t>
-  </si>
-  <si>
-    <t>plot_azmp_physical(mpa=MPAs,parameter="chlorophyll", type="surface")</t>
-  </si>
-  <si>
-    <t>plot_azmp_physical(mpa=MPAs,parameter="temperature", type="surface", dataframe=TRUE)</t>
-  </si>
-  <si>
-    <t>plot_azmp_physical(mpa=MPAs, type=NULL, parameter="sea_surface_height")</t>
-  </si>
-  <si>
     <t>Mean temperature of catch</t>
   </si>
   <si>
-    <t>plot_azmp_physical(mpa=MPAs, type=NULL, parameter="Zooplankton")</t>
+    <t>plot_trend_status(mpa=MPAs, type=NULL, parameter="Zooplankton")</t>
+  </si>
+  <si>
+    <t>plot_trend_status(mpa=MPAs,parameter="nitrate", type="surface")</t>
+  </si>
+  <si>
+    <t>plot_trend_status(mpa=MPAs,parameter="salinity", type="surface", dataframe=TRUE)</t>
+  </si>
+  <si>
+    <t>plot_trend_status(mpa=MPAs,parameter="chlorophyll", type="surface")</t>
+  </si>
+  <si>
+    <t>plot_trend_status(mpa=MPAs,parameter="temperature", type="surface", dataframe=TRUE)</t>
+  </si>
+  <si>
+    <t>plot_trend_status(mpa=MPAs, type=NULL, parameter="sea_surface_height")</t>
+  </si>
+  <si>
+    <t>Fish Condition Length</t>
+  </si>
+  <si>
+    <t>Fish Condition Weight</t>
+  </si>
+  <si>
+    <t>plot_trend_status(mpa=MPAs, area="Western/Emerald Banks Conservation Area (Restricted Fisheries Zone)", type=NULL, parameter="fish_weight", GS=gsdet)</t>
+  </si>
+  <si>
+    <t>plot_trend_status(mpa=MPAs, area="Western/Emerald Banks Conservation Area (Restricted Fisheries Zone)", type=NULL, parameter="fish_length", GS=gsdet)</t>
+  </si>
+  <si>
+    <t>plot_trend_status(mpa=MPAs, area="Western/Emerald Banks Conservation Area (Restricted Fisheries Zone)", type=NULL, parameter="haddock_abundance")</t>
+  </si>
+  <si>
+    <t>plot_trend_status(mpa=MPAs, area="Western/Emerald Banks Conservation Area (Restricted Fisheries Zone)", type=NULL, parameter="haddock_biomass")</t>
+  </si>
+  <si>
+    <t>plot_trend_status(mpa=MPAs,parameter="bloom_amplitude", type="surface")</t>
   </si>
 </sst>
 </file>
@@ -963,12 +981,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F115"/>
+  <dimension ref="A1:F116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A68" sqref="A68"/>
-      <selection pane="topRight" activeCell="F68" sqref="F68"/>
+      <selection pane="topRight" activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -993,10 +1011,10 @@
         <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1016,7 +1034,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1036,7 +1054,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -1056,7 +1074,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -1076,7 +1094,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1096,7 +1114,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -1116,7 +1134,7 @@
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -1136,7 +1154,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -1156,7 +1174,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -1176,7 +1194,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -1196,7 +1214,7 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1216,7 +1234,7 @@
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -1236,7 +1254,7 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -1256,7 +1274,7 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -1276,7 +1294,7 @@
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -1296,7 +1314,7 @@
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -1316,7 +1334,7 @@
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -1336,7 +1354,7 @@
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -1356,7 +1374,7 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -1376,7 +1394,7 @@
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -1396,7 +1414,7 @@
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1416,7 +1434,7 @@
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
@@ -1436,7 +1454,7 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
@@ -1456,7 +1474,7 @@
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
@@ -1476,7 +1494,7 @@
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
@@ -1496,7 +1514,7 @@
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
@@ -1516,7 +1534,7 @@
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
@@ -1536,7 +1554,7 @@
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
@@ -1556,7 +1574,7 @@
         <v>0</v>
       </c>
       <c r="F29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
@@ -1576,7 +1594,7 @@
         <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
@@ -1596,7 +1614,7 @@
         <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
@@ -1616,7 +1634,7 @@
         <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
@@ -1636,7 +1654,7 @@
         <v>0</v>
       </c>
       <c r="F33" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
@@ -1656,7 +1674,7 @@
         <v>0</v>
       </c>
       <c r="F34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
@@ -1676,7 +1694,7 @@
         <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
@@ -1696,7 +1714,7 @@
         <v>0</v>
       </c>
       <c r="F36" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
@@ -1716,7 +1734,7 @@
         <v>0</v>
       </c>
       <c r="F37" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
@@ -1736,7 +1754,7 @@
         <v>0</v>
       </c>
       <c r="F38" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
@@ -1756,7 +1774,7 @@
         <v>0</v>
       </c>
       <c r="F39" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
@@ -1776,7 +1794,7 @@
         <v>0</v>
       </c>
       <c r="F40" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
@@ -1796,7 +1814,7 @@
         <v>0</v>
       </c>
       <c r="F41" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
@@ -1816,7 +1834,7 @@
         <v>0</v>
       </c>
       <c r="F42" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
@@ -1836,7 +1854,7 @@
         <v>0</v>
       </c>
       <c r="F43" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
@@ -1856,7 +1874,7 @@
         <v>0</v>
       </c>
       <c r="F44" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
@@ -1876,7 +1894,7 @@
         <v>0</v>
       </c>
       <c r="F45" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
@@ -1896,7 +1914,7 @@
         <v>0</v>
       </c>
       <c r="F46" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
@@ -1916,7 +1934,7 @@
         <v>0</v>
       </c>
       <c r="F47" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
@@ -1936,7 +1954,7 @@
         <v>0</v>
       </c>
       <c r="F48" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
@@ -1956,7 +1974,7 @@
         <v>0</v>
       </c>
       <c r="F49" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
@@ -1976,7 +1994,7 @@
         <v>0</v>
       </c>
       <c r="F50" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
@@ -1996,7 +2014,7 @@
         <v>0</v>
       </c>
       <c r="F51" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
@@ -2016,7 +2034,7 @@
         <v>0</v>
       </c>
       <c r="F52" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
@@ -2036,7 +2054,7 @@
         <v>0</v>
       </c>
       <c r="F53" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
@@ -2056,7 +2074,7 @@
         <v>0</v>
       </c>
       <c r="F54" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
@@ -2076,7 +2094,7 @@
         <v>0</v>
       </c>
       <c r="F55" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
@@ -2096,7 +2114,7 @@
         <v>0</v>
       </c>
       <c r="F56" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -2116,7 +2134,7 @@
         <v>0</v>
       </c>
       <c r="F57" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
@@ -2136,7 +2154,7 @@
         <v>0</v>
       </c>
       <c r="F58" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
@@ -2156,7 +2174,7 @@
         <v>0</v>
       </c>
       <c r="F59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
@@ -2176,7 +2194,7 @@
         <v>0</v>
       </c>
       <c r="F60" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
@@ -2196,7 +2214,7 @@
         <v>0</v>
       </c>
       <c r="F61" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
@@ -2216,7 +2234,7 @@
         <v>0</v>
       </c>
       <c r="F62" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
@@ -2236,7 +2254,7 @@
         <v>0</v>
       </c>
       <c r="F63" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
@@ -2256,7 +2274,7 @@
         <v>0</v>
       </c>
       <c r="F64" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
@@ -2276,7 +2294,7 @@
         <v>0</v>
       </c>
       <c r="F65" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
@@ -2296,7 +2314,7 @@
         <v>0</v>
       </c>
       <c r="F66" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="67" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -2316,172 +2334,172 @@
         <v>0</v>
       </c>
       <c r="F67" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="68" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="s">
-        <v>116</v>
+        <v>179</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E68">
         <v>0</v>
       </c>
-      <c r="F68" t="s">
-        <v>169</v>
+      <c r="F68" s="7" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="69" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69" s="4" t="s">
-        <v>117</v>
+        <v>178</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="E69">
-        <v>0</v>
+        <v>167</v>
+      </c>
+      <c r="E69" t="s">
+        <v>180</v>
       </c>
       <c r="F69" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="70" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E70">
-        <v>0</v>
+        <v>167</v>
+      </c>
+      <c r="E70" t="s">
+        <v>181</v>
       </c>
       <c r="F70" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="71" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="E71">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="E71" t="s">
+        <v>172</v>
       </c>
       <c r="F71" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="72" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>17</v>
+        <v>167</v>
       </c>
       <c r="E72">
         <v>0</v>
       </c>
       <c r="F72" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="73" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A73" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="E73">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="E73" t="s">
+        <v>183</v>
       </c>
       <c r="F73" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A74" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>28</v>
+        <v>161</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E74">
-        <v>0</v>
+        <v>167</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F74" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="75" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A75" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="E75" s="9" t="s">
-        <v>172</v>
+        <v>15</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
       </c>
       <c r="F75" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="76" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A76" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>59</v>
@@ -2490,18 +2508,18 @@
         <v>14</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="E76">
-        <v>0</v>
+        <v>167</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>173</v>
       </c>
       <c r="F76" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A77" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>59</v>
@@ -2510,18 +2528,18 @@
         <v>14</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="E77" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
       </c>
       <c r="F77" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="78" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A78" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>59</v>
@@ -2530,18 +2548,18 @@
         <v>14</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="E78">
-        <v>0</v>
+        <v>167</v>
+      </c>
+      <c r="E78" s="9" t="s">
+        <v>174</v>
       </c>
       <c r="F78" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="79" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>59</v>
@@ -2550,18 +2568,18 @@
         <v>14</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>15</v>
+        <v>167</v>
       </c>
       <c r="E79">
         <v>0</v>
       </c>
       <c r="F79" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="80" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A80" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>59</v>
@@ -2570,18 +2588,18 @@
         <v>14</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>168</v>
+        <v>15</v>
       </c>
       <c r="E80">
         <v>0</v>
       </c>
       <c r="F80" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="81" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A81" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>59</v>
@@ -2590,18 +2608,18 @@
         <v>14</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E81">
         <v>0</v>
       </c>
       <c r="F81" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="82" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A82" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>59</v>
@@ -2610,18 +2628,18 @@
         <v>14</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E82" s="9" t="s">
-        <v>174</v>
+        <v>167</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
       </c>
       <c r="F82" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="83" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A83" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>59</v>
@@ -2632,16 +2650,16 @@
       <c r="D83" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E83">
-        <v>0</v>
+      <c r="E83" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="F83" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="84" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A84" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B84" s="5" t="s">
         <v>59</v>
@@ -2650,44 +2668,44 @@
         <v>14</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="E84">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="E84" t="s">
+        <v>184</v>
       </c>
       <c r="F84" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="85" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A85" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>163</v>
+        <v>14</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>59</v>
+        <v>167</v>
       </c>
       <c r="E85">
         <v>0</v>
       </c>
       <c r="F85" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="86" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>59</v>
@@ -2696,18 +2714,18 @@
         <v>0</v>
       </c>
       <c r="F86" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="87" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A87" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D87" s="6" t="s">
         <v>59</v>
@@ -2716,252 +2734,252 @@
         <v>0</v>
       </c>
       <c r="F87" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="88" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B88" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>168</v>
+        <v>59</v>
       </c>
       <c r="E88">
         <v>0</v>
       </c>
       <c r="F88" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="89" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A89" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B89" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>37</v>
+        <v>162</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E89">
         <v>0</v>
       </c>
       <c r="F89" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="90" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A90" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>164</v>
+        <v>37</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>15</v>
+        <v>167</v>
       </c>
       <c r="E90">
         <v>0</v>
       </c>
       <c r="F90" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="91" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A91" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B91" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E91">
         <v>0</v>
       </c>
       <c r="F91" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="92" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A92" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B92" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>168</v>
+        <v>17</v>
       </c>
       <c r="E92">
         <v>0</v>
       </c>
       <c r="F92" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="93" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A93" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B93" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E93" s="9">
+        <v>167</v>
+      </c>
+      <c r="E93">
         <v>0</v>
       </c>
       <c r="F93" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="94" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A94" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B94" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="E94">
+        <v>15</v>
+      </c>
+      <c r="E94" s="9">
         <v>0</v>
       </c>
       <c r="F94" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="95" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A95" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B95" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E95">
         <v>0</v>
       </c>
       <c r="F95" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="96" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A96" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B96" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C96" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D96" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="D96" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="E96" s="9" t="s">
-        <v>175</v>
+      <c r="E96">
+        <v>0</v>
       </c>
       <c r="F96" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="97" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A97" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B97" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>37</v>
+        <v>166</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="E97">
-        <v>0</v>
+        <v>167</v>
+      </c>
+      <c r="E97" s="9" t="s">
+        <v>176</v>
       </c>
       <c r="F97" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="98" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A98" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B98" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>165</v>
+        <v>37</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E98">
         <v>0</v>
       </c>
       <c r="F98" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="99" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B99" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>33</v>
+        <v>164</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E99">
         <v>0</v>
       </c>
       <c r="F99" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="100" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A100" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B100" s="5" t="s">
         <v>59</v>
@@ -2970,18 +2988,18 @@
         <v>33</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E100">
         <v>0</v>
       </c>
       <c r="F100" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="101" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A101" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B101" s="5" t="s">
         <v>59</v>
@@ -2990,18 +3008,18 @@
         <v>33</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>59</v>
+        <v>167</v>
       </c>
       <c r="E101">
         <v>0</v>
       </c>
       <c r="F101" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="102" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A102" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B102" s="5" t="s">
         <v>59</v>
@@ -3010,58 +3028,58 @@
         <v>33</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="E102">
         <v>0</v>
       </c>
       <c r="F102" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="103" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A103" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B103" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>166</v>
+        <v>33</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>168</v>
+        <v>15</v>
       </c>
       <c r="E103">
         <v>0</v>
       </c>
       <c r="F103" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="104" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A104" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B104" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>37</v>
+        <v>165</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E104">
         <v>0</v>
       </c>
       <c r="F104" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="105" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A105" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B105" s="5" t="s">
         <v>59</v>
@@ -3070,18 +3088,18 @@
         <v>37</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E105">
         <v>0</v>
       </c>
       <c r="F105" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="106" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A106" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B106" s="5" t="s">
         <v>59</v>
@@ -3090,18 +3108,18 @@
         <v>37</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>17</v>
+        <v>167</v>
       </c>
       <c r="E106">
         <v>0</v>
       </c>
       <c r="F106" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="107" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A107" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B107" s="5" t="s">
         <v>59</v>
@@ -3110,18 +3128,18 @@
         <v>37</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E107">
         <v>0</v>
       </c>
       <c r="F107" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="108" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A108" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B108" s="5" t="s">
         <v>59</v>
@@ -3136,12 +3154,12 @@
         <v>0</v>
       </c>
       <c r="F108" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="109" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A109" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B109" s="5" t="s">
         <v>59</v>
@@ -3150,18 +3168,18 @@
         <v>37</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="E109">
         <v>0</v>
       </c>
       <c r="F109" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="110" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A110" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B110" s="5" t="s">
         <v>59</v>
@@ -3170,18 +3188,18 @@
         <v>37</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="E110">
         <v>0</v>
       </c>
       <c r="F110" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="111" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A111" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B111" s="5" t="s">
         <v>59</v>
@@ -3190,93 +3208,113 @@
         <v>37</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>168</v>
+        <v>15</v>
       </c>
       <c r="E111">
         <v>0</v>
       </c>
       <c r="F111" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="112" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A112" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B112" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C112" s="7" t="s">
+      <c r="C112" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D112" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="E112">
+        <v>0</v>
+      </c>
+      <c r="F112" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A113" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C113" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D112" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="E112">
-        <v>0</v>
-      </c>
-      <c r="F112" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="8" t="s">
+      <c r="D113" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="E113">
+        <v>0</v>
+      </c>
+      <c r="F113" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A114" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C114" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D114" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E114" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="F114" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>60</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C115" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D115" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E115" s="9">
+        <v>0</v>
+      </c>
+      <c r="F115" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A116" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="B113" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C113" s="6" t="s">
+      <c r="B116" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C116" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D113" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E113" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="F113" s="7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A114" t="s">
-        <v>60</v>
-      </c>
-      <c r="B114" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C114" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D114" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E114" s="9">
-        <v>0</v>
-      </c>
-      <c r="F114" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A115" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="B115" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C115" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D115" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E115">
-        <v>0</v>
-      </c>
-      <c r="F115" s="7" t="s">
-        <v>169</v>
+      <c r="D116" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E116">
+        <v>0</v>
+      </c>
+      <c r="F116" s="7" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
whale bio + fix uu
</commit_message>
<xml_diff>
--- a/data/indicator_binning.xlsx
+++ b/data/indicator_binning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HarbinJ\Documents\GitHub\MarConsNetAnalysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA3828A-036B-48BE-8D7A-B9A8AE76A046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1CE92B-2ED9-4AEE-89C3-FA2A18F3A20A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -619,7 +619,7 @@
     <t>direct</t>
   </si>
   <si>
-    <t>plot_trend_status(df=whale_sighting, mpa=MPAs, type=NULL, parameter="whale_sightings")</t>
+    <t>plot_trend_status(df=whale_biodiversity, mpa=MPAs, type=NULL, parameter="whale_sightings")</t>
   </si>
 </sst>
 </file>
@@ -1034,9 +1034,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F113" sqref="F113"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N110" sqref="N110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
streamline add data to app
</commit_message>
<xml_diff>
--- a/data/indicator_binning.xlsx
+++ b/data/indicator_binning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HarbinJ\Documents\GitHub\MarConsNetAnalysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8307D906-C1B8-4641-AB3C-CC5F3AA3B2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CF28F1-BBDD-45FB-A0FB-200BFBE87E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -565,39 +565,6 @@
     <t>project</t>
   </si>
   <si>
-    <t>plot_trend_status(df=gsdet, mpa=MPAs, area="Western/Emerald Banks Conservation Area (Restricted Fisheries Zone)", type=NULL, parameter="fish_weight")</t>
-  </si>
-  <si>
-    <t>plot_trend_status(df=gsdet, mpa=MPAs, area="Western/Emerald Banks Conservation Area (Restricted Fisheries Zone)", type=NULL, parameter="fish_length")</t>
-  </si>
-  <si>
-    <t>plot_trend_status(df=zooplankton, mpa=MPAs, type=NULL, parameter="Zooplankton")</t>
-  </si>
-  <si>
-    <t>plot_trend_status(df=all_haddock, mpa=MPAs, area="Western/Emerald Banks Conservation Area (Restricted Fisheries Zone)", type=NULL, parameter="haddock_biomass")</t>
-  </si>
-  <si>
-    <t>plot_trend_status(df=all_haddock, mpa=MPAs, area="Western/Emerald Banks Conservation Area (Restricted Fisheries Zone)", type=NULL, parameter="haddock_abundance")</t>
-  </si>
-  <si>
-    <t>plot_trend_status(df=bloom_df, mpa=MPAs,parameter="bloom_amplitude", type="surface")</t>
-  </si>
-  <si>
-    <t>plot_trend_status(df=azmpdata::Discrete_Occupations_Sections, mpa=MPAs,parameter="salinity", type="surface", dataframe=TRUE)</t>
-  </si>
-  <si>
-    <t>plot_trend_status(df=azmpdata::Discrete_Occupations_Sections, mpa=MPAs,parameter="chlorophyll", type="surface")</t>
-  </si>
-  <si>
-    <t>plot_trend_status(df=azmpdata::Discrete_Occupations_Sections, mpa=MPAs,parameter="temperature", type="surface", dataframe=TRUE)</t>
-  </si>
-  <si>
-    <t>plot_trend_status(df=surface_height, mpa=MPAs, type=NULL, parameter="sea_surface_height")</t>
-  </si>
-  <si>
-    <t>plot_trend_status(df=azmpdata::Discrete_Occupations_Sections, mpa=MPAs,parameter="nitrate", type="surface")</t>
-  </si>
-  <si>
     <t>mpa_name</t>
   </si>
   <si>
@@ -619,7 +586,40 @@
     <t>direct</t>
   </si>
   <si>
-    <t>plot_trend_status(df=whale_biodiversity, mpa=MPAs, type=NULL, parameter="whale_biodiversity")</t>
+    <t>plot_trend_status(df=bloom_df, mpa=MPAs, type="surface")</t>
+  </si>
+  <si>
+    <t>plot_trend_status(df=zooplankton, mpa=MPAs, type=NULL)</t>
+  </si>
+  <si>
+    <t>plot_trend_status(df=whale_biodiversity, mpa=MPAs, type=NULL)</t>
+  </si>
+  <si>
+    <t>plot_trend_status(df=surface_height, mpa=MPAs, type=NULL)</t>
+  </si>
+  <si>
+    <t>plot_trend_status(df=all_haddock, mpa=MPAs, area="Western/Emerald Banks Conservation Area (Restricted Fisheries Zone)", type=NULL)</t>
+  </si>
+  <si>
+    <t>plot_trend_status(df=fish_weight, mpa=MPAs, area="Western/Emerald Banks Conservation Area (Restricted Fisheries Zone)", type=NULL)</t>
+  </si>
+  <si>
+    <t>plot_trend_status(df=fish_length, mpa=MPAs, area="Western/Emerald Banks Conservation Area (Restricted Fisheries Zone)", type=NULL)</t>
+  </si>
+  <si>
+    <t>plot_trend_status(df=haddock_biomass, mpa=MPAs, area="Western/Emerald Banks Conservation Area (Restricted Fisheries Zone)", type=NULL)</t>
+  </si>
+  <si>
+    <t>plot_trend_status(df=nitrate, mpa=MPAs, type="surface")</t>
+  </si>
+  <si>
+    <t>plot_trend_status(df=salinity, mpa=MPAs, type="surface", dataframe=TRUE)</t>
+  </si>
+  <si>
+    <t>plot_trend_status(df=chlorophyll, mpa=MPAs, type="surface")</t>
+  </si>
+  <si>
+    <t>plot_trend_status(df=temperature, mpa=MPAs, type="surface", dataframe=TRUE)</t>
   </si>
 </sst>
 </file>
@@ -1034,9 +1034,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F113" sqref="F113"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1052,7 +1052,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1076,7 +1076,7 @@
         <v>179</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -1084,7 +1084,7 @@
         <v>62</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -1108,7 +1108,7 @@
         <v>179</v>
       </c>
       <c r="J2" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -1116,7 +1116,7 @@
         <v>63</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -1140,7 +1140,7 @@
         <v>179</v>
       </c>
       <c r="J3" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -1148,7 +1148,7 @@
         <v>64</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -1172,7 +1172,7 @@
         <v>179</v>
       </c>
       <c r="J4" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -1180,7 +1180,7 @@
         <v>65</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -1204,7 +1204,7 @@
         <v>179</v>
       </c>
       <c r="J5" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -1212,7 +1212,7 @@
         <v>66</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -1236,7 +1236,7 @@
         <v>179</v>
       </c>
       <c r="J6" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -1244,7 +1244,7 @@
         <v>67</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -1268,7 +1268,7 @@
         <v>179</v>
       </c>
       <c r="J7" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -1276,7 +1276,7 @@
         <v>68</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -1300,7 +1300,7 @@
         <v>179</v>
       </c>
       <c r="J8" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -1308,7 +1308,7 @@
         <v>69</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
@@ -1332,7 +1332,7 @@
         <v>179</v>
       </c>
       <c r="J9" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -1340,7 +1340,7 @@
         <v>70</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
@@ -1364,7 +1364,7 @@
         <v>179</v>
       </c>
       <c r="J10" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -1372,7 +1372,7 @@
         <v>71</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -1396,7 +1396,7 @@
         <v>179</v>
       </c>
       <c r="J11" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1404,7 +1404,7 @@
         <v>72</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>2</v>
@@ -1428,7 +1428,7 @@
         <v>179</v>
       </c>
       <c r="J12" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K12"/>
     </row>
@@ -1437,7 +1437,7 @@
         <v>73</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
@@ -1461,7 +1461,7 @@
         <v>179</v>
       </c>
       <c r="J13" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -1469,7 +1469,7 @@
         <v>74</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
@@ -1493,7 +1493,7 @@
         <v>179</v>
       </c>
       <c r="J14" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
@@ -1501,7 +1501,7 @@
         <v>75</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
@@ -1525,7 +1525,7 @@
         <v>179</v>
       </c>
       <c r="J15" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
@@ -1533,7 +1533,7 @@
         <v>76</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
@@ -1557,7 +1557,7 @@
         <v>179</v>
       </c>
       <c r="J16" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
@@ -1565,7 +1565,7 @@
         <v>77</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -1589,7 +1589,7 @@
         <v>179</v>
       </c>
       <c r="J17" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
@@ -1597,7 +1597,7 @@
         <v>78</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
@@ -1621,7 +1621,7 @@
         <v>179</v>
       </c>
       <c r="J18" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
@@ -1629,7 +1629,7 @@
         <v>79</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
@@ -1653,7 +1653,7 @@
         <v>179</v>
       </c>
       <c r="J19" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
@@ -1661,7 +1661,7 @@
         <v>80</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
@@ -1685,7 +1685,7 @@
         <v>179</v>
       </c>
       <c r="J20" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
@@ -1693,7 +1693,7 @@
         <v>81</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -1717,7 +1717,7 @@
         <v>179</v>
       </c>
       <c r="J21" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1725,7 +1725,7 @@
         <v>82</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>2</v>
@@ -1749,7 +1749,7 @@
         <v>179</v>
       </c>
       <c r="J22" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K22"/>
     </row>
@@ -1758,7 +1758,7 @@
         <v>83</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
@@ -1782,7 +1782,7 @@
         <v>179</v>
       </c>
       <c r="J23" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
@@ -1790,7 +1790,7 @@
         <v>84</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
@@ -1814,7 +1814,7 @@
         <v>179</v>
       </c>
       <c r="J24" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
@@ -1822,7 +1822,7 @@
         <v>85</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
@@ -1846,7 +1846,7 @@
         <v>179</v>
       </c>
       <c r="J25" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
@@ -1854,7 +1854,7 @@
         <v>86</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C26" t="s">
         <v>2</v>
@@ -1878,7 +1878,7 @@
         <v>179</v>
       </c>
       <c r="J26" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
@@ -1886,7 +1886,7 @@
         <v>87</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C27" t="s">
         <v>2</v>
@@ -1910,7 +1910,7 @@
         <v>179</v>
       </c>
       <c r="J27" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
@@ -1918,7 +1918,7 @@
         <v>88</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C28" t="s">
         <v>3</v>
@@ -1942,7 +1942,7 @@
         <v>179</v>
       </c>
       <c r="J28" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
@@ -1950,7 +1950,7 @@
         <v>89</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C29" t="s">
         <v>3</v>
@@ -1974,7 +1974,7 @@
         <v>179</v>
       </c>
       <c r="J29" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
@@ -1982,7 +1982,7 @@
         <v>90</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C30" t="s">
         <v>3</v>
@@ -2006,7 +2006,7 @@
         <v>179</v>
       </c>
       <c r="J30" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
@@ -2014,7 +2014,7 @@
         <v>91</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C31" t="s">
         <v>3</v>
@@ -2038,7 +2038,7 @@
         <v>179</v>
       </c>
       <c r="J31" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
@@ -2046,7 +2046,7 @@
         <v>92</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C32" t="s">
         <v>3</v>
@@ -2070,7 +2070,7 @@
         <v>179</v>
       </c>
       <c r="J32" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
@@ -2078,7 +2078,7 @@
         <v>93</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C33" t="s">
         <v>3</v>
@@ -2102,7 +2102,7 @@
         <v>179</v>
       </c>
       <c r="J33" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
@@ -2110,7 +2110,7 @@
         <v>94</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C34" t="s">
         <v>3</v>
@@ -2134,7 +2134,7 @@
         <v>179</v>
       </c>
       <c r="J34" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
@@ -2142,7 +2142,7 @@
         <v>95</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C35" t="s">
         <v>3</v>
@@ -2166,7 +2166,7 @@
         <v>179</v>
       </c>
       <c r="J35" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
@@ -2174,7 +2174,7 @@
         <v>96</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C36" t="s">
         <v>3</v>
@@ -2198,7 +2198,7 @@
         <v>179</v>
       </c>
       <c r="J36" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
@@ -2206,7 +2206,7 @@
         <v>97</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C37" t="s">
         <v>3</v>
@@ -2230,7 +2230,7 @@
         <v>179</v>
       </c>
       <c r="J37" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
@@ -2238,7 +2238,7 @@
         <v>98</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C38" t="s">
         <v>3</v>
@@ -2262,7 +2262,7 @@
         <v>179</v>
       </c>
       <c r="J38" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
@@ -2270,7 +2270,7 @@
         <v>99</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C39" t="s">
         <v>3</v>
@@ -2294,7 +2294,7 @@
         <v>179</v>
       </c>
       <c r="J39" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
@@ -2302,7 +2302,7 @@
         <v>100</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C40" t="s">
         <v>3</v>
@@ -2326,7 +2326,7 @@
         <v>179</v>
       </c>
       <c r="J40" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
@@ -2334,7 +2334,7 @@
         <v>101</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C41" t="s">
         <v>3</v>
@@ -2358,7 +2358,7 @@
         <v>179</v>
       </c>
       <c r="J41" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
@@ -2366,7 +2366,7 @@
         <v>102</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C42" t="s">
         <v>3</v>
@@ -2390,7 +2390,7 @@
         <v>179</v>
       </c>
       <c r="J42" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
@@ -2398,7 +2398,7 @@
         <v>103</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C43" t="s">
         <v>3</v>
@@ -2422,7 +2422,7 @@
         <v>179</v>
       </c>
       <c r="J43" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.35">
@@ -2430,7 +2430,7 @@
         <v>104</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C44" t="s">
         <v>3</v>
@@ -2454,7 +2454,7 @@
         <v>179</v>
       </c>
       <c r="J44" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.35">
@@ -2462,7 +2462,7 @@
         <v>105</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C45" t="s">
         <v>3</v>
@@ -2486,7 +2486,7 @@
         <v>179</v>
       </c>
       <c r="J45" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.35">
@@ -2494,7 +2494,7 @@
         <v>106</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C46" t="s">
         <v>3</v>
@@ -2518,7 +2518,7 @@
         <v>179</v>
       </c>
       <c r="J46" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
@@ -2526,7 +2526,7 @@
         <v>107</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C47" t="s">
         <v>3</v>
@@ -2550,7 +2550,7 @@
         <v>179</v>
       </c>
       <c r="J47" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.35">
@@ -2558,7 +2558,7 @@
         <v>108</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C48" t="s">
         <v>3</v>
@@ -2582,7 +2582,7 @@
         <v>179</v>
       </c>
       <c r="J48" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.35">
@@ -2590,7 +2590,7 @@
         <v>109</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C49" t="s">
         <v>3</v>
@@ -2614,7 +2614,7 @@
         <v>179</v>
       </c>
       <c r="J49" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.35">
@@ -2622,7 +2622,7 @@
         <v>110</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C50" t="s">
         <v>3</v>
@@ -2646,7 +2646,7 @@
         <v>179</v>
       </c>
       <c r="J50" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.35">
@@ -2654,7 +2654,7 @@
         <v>111</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C51" t="s">
         <v>3</v>
@@ -2678,7 +2678,7 @@
         <v>179</v>
       </c>
       <c r="J51" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.35">
@@ -2686,7 +2686,7 @@
         <v>112</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C52" t="s">
         <v>3</v>
@@ -2710,7 +2710,7 @@
         <v>179</v>
       </c>
       <c r="J52" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.35">
@@ -2718,7 +2718,7 @@
         <v>113</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C53" t="s">
         <v>3</v>
@@ -2742,7 +2742,7 @@
         <v>179</v>
       </c>
       <c r="J53" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.35">
@@ -2750,7 +2750,7 @@
         <v>114</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C54" t="s">
         <v>3</v>
@@ -2774,7 +2774,7 @@
         <v>179</v>
       </c>
       <c r="J54" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.35">
@@ -2782,7 +2782,7 @@
         <v>115</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C55" t="s">
         <v>3</v>
@@ -2806,7 +2806,7 @@
         <v>179</v>
       </c>
       <c r="J55" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.35">
@@ -2814,7 +2814,7 @@
         <v>4</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="C56" t="s">
         <v>5</v>
@@ -2838,7 +2838,7 @@
         <v>179</v>
       </c>
       <c r="J56" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -2846,7 +2846,7 @@
         <v>48</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="C57" t="s">
         <v>5</v>
@@ -2870,7 +2870,7 @@
         <v>179</v>
       </c>
       <c r="J57" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.35">
@@ -2878,7 +2878,7 @@
         <v>51</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="C58" t="s">
         <v>5</v>
@@ -2902,7 +2902,7 @@
         <v>179</v>
       </c>
       <c r="J58" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.35">
@@ -2910,7 +2910,7 @@
         <v>50</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="C59" t="s">
         <v>5</v>
@@ -2934,7 +2934,7 @@
         <v>179</v>
       </c>
       <c r="J59" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.35">
@@ -2942,7 +2942,7 @@
         <v>53</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="C60" t="s">
         <v>5</v>
@@ -2966,7 +2966,7 @@
         <v>179</v>
       </c>
       <c r="J60" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.35">
@@ -2974,7 +2974,7 @@
         <v>6</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="C61" t="s">
         <v>5</v>
@@ -2998,7 +2998,7 @@
         <v>179</v>
       </c>
       <c r="J61" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.35">
@@ -3006,7 +3006,7 @@
         <v>7</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="C62" t="s">
         <v>5</v>
@@ -3030,7 +3030,7 @@
         <v>179</v>
       </c>
       <c r="J62" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.35">
@@ -3038,7 +3038,7 @@
         <v>8</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="C63" t="s">
         <v>5</v>
@@ -3062,7 +3062,7 @@
         <v>179</v>
       </c>
       <c r="J63" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.35">
@@ -3070,7 +3070,7 @@
         <v>9</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="C64" t="s">
         <v>5</v>
@@ -3094,7 +3094,7 @@
         <v>179</v>
       </c>
       <c r="J64" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.35">
@@ -3102,7 +3102,7 @@
         <v>56</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="C65" t="s">
         <v>5</v>
@@ -3126,7 +3126,7 @@
         <v>179</v>
       </c>
       <c r="J65" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.35">
@@ -3134,7 +3134,7 @@
         <v>10</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="C66" t="s">
         <v>5</v>
@@ -3158,7 +3158,7 @@
         <v>179</v>
       </c>
       <c r="J66" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="67" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -3166,7 +3166,7 @@
         <v>11</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>5</v>
@@ -3190,7 +3190,7 @@
         <v>179</v>
       </c>
       <c r="J67" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K67"/>
     </row>
@@ -3199,7 +3199,7 @@
         <v>172</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>59</v>
@@ -3211,7 +3211,7 @@
         <v>166</v>
       </c>
       <c r="F68" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="G68" s="7" t="s">
         <v>167</v>
@@ -3223,7 +3223,7 @@
         <v>726</v>
       </c>
       <c r="J68" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K68"/>
     </row>
@@ -3232,7 +3232,7 @@
         <v>171</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>59</v>
@@ -3244,7 +3244,7 @@
         <v>166</v>
       </c>
       <c r="F69" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="G69" t="s">
         <v>167</v>
@@ -3256,7 +3256,7 @@
         <v>726</v>
       </c>
       <c r="J69" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K69"/>
     </row>
@@ -3265,7 +3265,7 @@
         <v>116</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>59</v>
@@ -3289,7 +3289,7 @@
         <v>179</v>
       </c>
       <c r="J70" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K70"/>
     </row>
@@ -3298,7 +3298,7 @@
         <v>117</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>59</v>
@@ -3310,7 +3310,7 @@
         <v>15</v>
       </c>
       <c r="F71" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="G71" t="s">
         <v>167</v>
@@ -3322,7 +3322,7 @@
         <v>579</v>
       </c>
       <c r="J71" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K71"/>
     </row>
@@ -3331,7 +3331,7 @@
         <v>118</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>59</v>
@@ -3355,7 +3355,7 @@
         <v>179</v>
       </c>
       <c r="J72" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K72"/>
     </row>
@@ -3364,7 +3364,7 @@
         <v>119</v>
       </c>
       <c r="B73" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>59</v>
@@ -3376,7 +3376,7 @@
         <v>17</v>
       </c>
       <c r="F73" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="G73" t="s">
         <v>167</v>
@@ -3388,7 +3388,7 @@
         <v>726</v>
       </c>
       <c r="J73" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K73"/>
     </row>
@@ -3397,7 +3397,7 @@
         <v>120</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>59</v>
@@ -3409,7 +3409,7 @@
         <v>166</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="G74" t="s">
         <v>167</v>
@@ -3421,7 +3421,7 @@
         <v>726</v>
       </c>
       <c r="J74" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K74"/>
     </row>
@@ -3430,7 +3430,7 @@
         <v>121</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>59</v>
@@ -3454,7 +3454,7 @@
         <v>179</v>
       </c>
       <c r="J75" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K75"/>
     </row>
@@ -3463,7 +3463,7 @@
         <v>122</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>59</v>
@@ -3475,7 +3475,7 @@
         <v>166</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="G76" t="s">
         <v>167</v>
@@ -3487,7 +3487,7 @@
         <v>579</v>
       </c>
       <c r="J76" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="K76"/>
     </row>
@@ -3496,7 +3496,7 @@
         <v>123</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>59</v>
@@ -3520,7 +3520,7 @@
         <v>179</v>
       </c>
       <c r="J77" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="K77"/>
     </row>
@@ -3529,7 +3529,7 @@
         <v>124</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>59</v>
@@ -3541,7 +3541,7 @@
         <v>166</v>
       </c>
       <c r="F78" s="9" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="G78" t="s">
         <v>167</v>
@@ -3553,7 +3553,7 @@
         <v>579</v>
       </c>
       <c r="J78" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K78"/>
     </row>
@@ -3562,7 +3562,7 @@
         <v>125</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>59</v>
@@ -3586,7 +3586,7 @@
         <v>179</v>
       </c>
       <c r="J79" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K79"/>
     </row>
@@ -3595,7 +3595,7 @@
         <v>126</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>59</v>
@@ -3619,7 +3619,7 @@
         <v>179</v>
       </c>
       <c r="J80" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K80"/>
     </row>
@@ -3628,7 +3628,7 @@
         <v>127</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C81" s="5" t="s">
         <v>59</v>
@@ -3652,7 +3652,7 @@
         <v>179</v>
       </c>
       <c r="J81" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="K81"/>
     </row>
@@ -3661,7 +3661,7 @@
         <v>128</v>
       </c>
       <c r="B82" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C82" s="5" t="s">
         <v>59</v>
@@ -3685,7 +3685,7 @@
         <v>179</v>
       </c>
       <c r="J82" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="K82"/>
     </row>
@@ -3694,7 +3694,7 @@
         <v>129</v>
       </c>
       <c r="B83" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C83" s="5" t="s">
         <v>59</v>
@@ -3706,7 +3706,7 @@
         <v>24</v>
       </c>
       <c r="F83" s="9" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="G83" t="s">
         <v>167</v>
@@ -3718,7 +3718,7 @@
         <v>579</v>
       </c>
       <c r="J83" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="K83"/>
     </row>
@@ -3727,7 +3727,7 @@
         <v>130</v>
       </c>
       <c r="B84" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C84" s="5" t="s">
         <v>59</v>
@@ -3739,7 +3739,7 @@
         <v>24</v>
       </c>
       <c r="F84" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="G84" t="s">
         <v>167</v>
@@ -3751,7 +3751,7 @@
         <v>579</v>
       </c>
       <c r="J84" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="K84"/>
     </row>
@@ -3760,7 +3760,7 @@
         <v>131</v>
       </c>
       <c r="B85" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C85" s="5" t="s">
         <v>59</v>
@@ -3784,7 +3784,7 @@
         <v>179</v>
       </c>
       <c r="J85" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K85"/>
     </row>
@@ -3793,7 +3793,7 @@
         <v>132</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C86" s="5" t="s">
         <v>59</v>
@@ -3817,7 +3817,7 @@
         <v>179</v>
       </c>
       <c r="J86" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K86"/>
     </row>
@@ -3826,7 +3826,7 @@
         <v>133</v>
       </c>
       <c r="B87" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C87" s="5" t="s">
         <v>59</v>
@@ -3850,7 +3850,7 @@
         <v>179</v>
       </c>
       <c r="J87" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K87"/>
     </row>
@@ -3859,7 +3859,7 @@
         <v>134</v>
       </c>
       <c r="B88" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C88" s="5" t="s">
         <v>59</v>
@@ -3883,7 +3883,7 @@
         <v>179</v>
       </c>
       <c r="J88" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K88"/>
     </row>
@@ -3892,7 +3892,7 @@
         <v>135</v>
       </c>
       <c r="B89" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C89" s="5" t="s">
         <v>59</v>
@@ -3916,7 +3916,7 @@
         <v>179</v>
       </c>
       <c r="J89" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K89"/>
     </row>
@@ -3925,7 +3925,7 @@
         <v>136</v>
       </c>
       <c r="B90" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C90" s="5" t="s">
         <v>59</v>
@@ -3949,7 +3949,7 @@
         <v>179</v>
       </c>
       <c r="J90" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K90"/>
     </row>
@@ -3958,7 +3958,7 @@
         <v>137</v>
       </c>
       <c r="B91" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C91" s="5" t="s">
         <v>59</v>
@@ -3982,7 +3982,7 @@
         <v>179</v>
       </c>
       <c r="J91" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K91"/>
     </row>
@@ -3991,7 +3991,7 @@
         <v>138</v>
       </c>
       <c r="B92" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C92" s="5" t="s">
         <v>59</v>
@@ -4015,7 +4015,7 @@
         <v>179</v>
       </c>
       <c r="J92" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K92"/>
     </row>
@@ -4024,7 +4024,7 @@
         <v>139</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C93" s="5" t="s">
         <v>59</v>
@@ -4048,7 +4048,7 @@
         <v>179</v>
       </c>
       <c r="J93" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K93"/>
     </row>
@@ -4057,7 +4057,7 @@
         <v>140</v>
       </c>
       <c r="B94" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C94" s="5" t="s">
         <v>59</v>
@@ -4081,7 +4081,7 @@
         <v>179</v>
       </c>
       <c r="J94" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K94"/>
     </row>
@@ -4090,7 +4090,7 @@
         <v>141</v>
       </c>
       <c r="B95" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C95" s="5" t="s">
         <v>59</v>
@@ -4114,7 +4114,7 @@
         <v>179</v>
       </c>
       <c r="J95" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K95"/>
     </row>
@@ -4123,7 +4123,7 @@
         <v>142</v>
       </c>
       <c r="B96" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C96" s="5" t="s">
         <v>59</v>
@@ -4147,7 +4147,7 @@
         <v>179</v>
       </c>
       <c r="J96" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K96"/>
     </row>
@@ -4156,7 +4156,7 @@
         <v>143</v>
       </c>
       <c r="B97" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C97" s="5" t="s">
         <v>59</v>
@@ -4168,7 +4168,7 @@
         <v>166</v>
       </c>
       <c r="F97" s="9" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="G97" t="s">
         <v>167</v>
@@ -4180,7 +4180,7 @@
         <v>579</v>
       </c>
       <c r="J97" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="K97"/>
     </row>
@@ -4189,7 +4189,7 @@
         <v>144</v>
       </c>
       <c r="B98" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C98" s="5" t="s">
         <v>59</v>
@@ -4213,7 +4213,7 @@
         <v>179</v>
       </c>
       <c r="J98" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K98"/>
     </row>
@@ -4222,7 +4222,7 @@
         <v>145</v>
       </c>
       <c r="B99" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C99" s="5" t="s">
         <v>59</v>
@@ -4246,7 +4246,7 @@
         <v>179</v>
       </c>
       <c r="J99" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K99"/>
     </row>
@@ -4255,7 +4255,7 @@
         <v>146</v>
       </c>
       <c r="B100" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C100" s="5" t="s">
         <v>59</v>
@@ -4279,7 +4279,7 @@
         <v>179</v>
       </c>
       <c r="J100" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K100"/>
     </row>
@@ -4288,7 +4288,7 @@
         <v>147</v>
       </c>
       <c r="B101" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C101" s="5" t="s">
         <v>59</v>
@@ -4312,7 +4312,7 @@
         <v>179</v>
       </c>
       <c r="J101" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K101"/>
     </row>
@@ -4321,7 +4321,7 @@
         <v>148</v>
       </c>
       <c r="B102" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C102" s="5" t="s">
         <v>59</v>
@@ -4345,7 +4345,7 @@
         <v>179</v>
       </c>
       <c r="J102" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K102"/>
     </row>
@@ -4354,7 +4354,7 @@
         <v>149</v>
       </c>
       <c r="B103" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C103" s="5" t="s">
         <v>59</v>
@@ -4378,7 +4378,7 @@
         <v>179</v>
       </c>
       <c r="J103" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K103"/>
     </row>
@@ -4387,7 +4387,7 @@
         <v>150</v>
       </c>
       <c r="B104" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C104" s="5" t="s">
         <v>59</v>
@@ -4411,7 +4411,7 @@
         <v>179</v>
       </c>
       <c r="J104" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K104"/>
     </row>
@@ -4420,7 +4420,7 @@
         <v>151</v>
       </c>
       <c r="B105" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C105" s="5" t="s">
         <v>59</v>
@@ -4444,7 +4444,7 @@
         <v>179</v>
       </c>
       <c r="J105" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K105"/>
     </row>
@@ -4453,7 +4453,7 @@
         <v>152</v>
       </c>
       <c r="B106" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C106" s="5" t="s">
         <v>59</v>
@@ -4477,7 +4477,7 @@
         <v>179</v>
       </c>
       <c r="J106" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K106"/>
     </row>
@@ -4486,7 +4486,7 @@
         <v>153</v>
       </c>
       <c r="B107" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C107" s="5" t="s">
         <v>59</v>
@@ -4510,7 +4510,7 @@
         <v>179</v>
       </c>
       <c r="J107" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K107"/>
     </row>
@@ -4519,7 +4519,7 @@
         <v>154</v>
       </c>
       <c r="B108" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C108" s="5" t="s">
         <v>59</v>
@@ -4543,7 +4543,7 @@
         <v>179</v>
       </c>
       <c r="J108" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K108"/>
     </row>
@@ -4552,7 +4552,7 @@
         <v>155</v>
       </c>
       <c r="B109" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C109" s="5" t="s">
         <v>59</v>
@@ -4576,7 +4576,7 @@
         <v>179</v>
       </c>
       <c r="J109" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K109"/>
     </row>
@@ -4585,7 +4585,7 @@
         <v>156</v>
       </c>
       <c r="B110" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C110" s="5" t="s">
         <v>59</v>
@@ -4609,7 +4609,7 @@
         <v>179</v>
       </c>
       <c r="J110" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K110"/>
     </row>
@@ -4618,7 +4618,7 @@
         <v>157</v>
       </c>
       <c r="B111" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C111" s="5" t="s">
         <v>59</v>
@@ -4642,7 +4642,7 @@
         <v>179</v>
       </c>
       <c r="J111" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K111"/>
     </row>
@@ -4651,7 +4651,7 @@
         <v>158</v>
       </c>
       <c r="B112" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C112" s="5" t="s">
         <v>59</v>
@@ -4675,7 +4675,7 @@
         <v>179</v>
       </c>
       <c r="J112" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K112"/>
     </row>
@@ -4684,7 +4684,7 @@
         <v>159</v>
       </c>
       <c r="B113" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C113" s="5" t="s">
         <v>59</v>
@@ -4696,7 +4696,7 @@
         <v>166</v>
       </c>
       <c r="F113" s="10" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="G113" t="s">
         <v>167</v>
@@ -4708,7 +4708,7 @@
         <v>1062</v>
       </c>
       <c r="J113" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K113"/>
     </row>
@@ -4717,7 +4717,7 @@
         <v>169</v>
       </c>
       <c r="B114" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C114" s="5" t="s">
         <v>59</v>
@@ -4729,7 +4729,7 @@
         <v>15</v>
       </c>
       <c r="F114" s="10" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G114" s="7" t="s">
         <v>167</v>
@@ -4741,7 +4741,7 @@
         <v>579</v>
       </c>
       <c r="J114" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="K114"/>
     </row>
@@ -4750,7 +4750,7 @@
         <v>60</v>
       </c>
       <c r="B115" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C115" s="5" t="s">
         <v>59</v>
@@ -4774,7 +4774,7 @@
         <v>179</v>
       </c>
       <c r="J115" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.35">
@@ -4782,7 +4782,7 @@
         <v>170</v>
       </c>
       <c r="B116" s="11" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C116" s="5" t="s">
         <v>59</v>
@@ -4806,7 +4806,7 @@
         <v>179</v>
       </c>
       <c r="J116" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>